<commit_message>
NB Reporting: - KZT Form 19 done (IFRS-9)
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_19.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_19.xlsx
@@ -19,9 +19,9 @@
     <definedName name="GR_CODE_SHEET">4</definedName>
     <definedName name="_xlnm.Database" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">РДХФИ_19!$A$1:$G$73</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">РДХФИ_19!$A$1:$G$46</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateCount="10000" iterateDelta="1E-10"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Код формы</t>
   </si>
@@ -75,11 +75,6 @@
     <t>Код строки</t>
   </si>
   <si>
-    <t>Национальный идентификационный 
-номер, международный 
-идентификационный номер, наименование контрагента для вкладов и займов</t>
-  </si>
-  <si>
     <t>Остаток на начало отчетного периода</t>
   </si>
   <si>
@@ -89,9 +84,6 @@
     <t>Остаток на конец отчетного периода (гр.5+гр.6)</t>
   </si>
   <si>
-    <t>Доходы в виде вознаграждения по размещенным вкладам (сумма строк 2-11)</t>
-  </si>
-  <si>
     <t>Доходы по вознаграждениям по вкладам до востребования</t>
   </si>
   <si>
@@ -104,188 +96,185 @@
     <t>Доходы по вознаграждениям по краткосрочным прочим вкладам</t>
   </si>
   <si>
-    <t>Доходы по вознаграждениям по долгосрочным прочим вкладам</t>
-  </si>
-  <si>
-    <t>Доходы по амортизации дисконта по вкладам до востребования</t>
-  </si>
-  <si>
     <t>Доходы по амортизации дисконта по краткосрочным срочным вкладам</t>
   </si>
   <si>
     <t>Доходы по амортизации дисконта по долгосрочным срочным вкладам</t>
   </si>
   <si>
-    <t>Доходы по амортизации дисконта по прочим краткосрочным вкладам</t>
-  </si>
-  <si>
-    <t>Доходы по амортизации дисконта по прочим долгосрочным вкладам</t>
-  </si>
-  <si>
-    <t>Доходы в виде вознаграждения по приобретенным ценным бумагам (сумма строк 13-21)</t>
-  </si>
-  <si>
-    <t>Доходы по вознаграждениям по краткосрочным финансовым инвестициям, оцениваемым по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка</t>
-  </si>
-  <si>
-    <t>Доходы по вознаграждениям по краткосрочным финансовым инвестициям, удерживаемым до погашения</t>
-  </si>
-  <si>
-    <t>Доходы по вознаграждениям по долгосрочным финансовым инвестициям, удерживаемым до погашения</t>
-  </si>
-  <si>
-    <t>Доходы по вознаграждениям по краткосрочным финансовым инвестициям, имеющимся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Доходы по вознаграждениям по долгосрочным финансовым инвестициям, имеющимся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Доходы по амортизации дисконта по краткосрочным финансовым инвестициям, удерживаемым до погашения</t>
-  </si>
-  <si>
-    <t>Доходы по амортизации дисконта по долгосрочным финансовым инвестициям, удерживаемым до погашения</t>
-  </si>
-  <si>
-    <t>Доходы по амортизации дисконта по краткосрочным финансовым инвестициям, имеющимся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Доходы по амортизации дисконта по долгосрочным финансовым инвестициям, имеющимся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Доходы (расходы) от купли-продажи ценных бумаг (сумма строк 23-28)</t>
-  </si>
-  <si>
-    <t>Доходы от покупки-продажи финансовых инвестиций, оцениваемых по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка</t>
-  </si>
-  <si>
-    <t>Доходы от покупки-продажи краткосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Доходы от покупки-продажи долгосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Расходы от покупки-продажи финансовых инвестиций, оцениваемых по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка</t>
-  </si>
-  <si>
-    <t>Расходы от покупки-продажи краткосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Расходы от покупки-продажи долгосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Доходы (расходы) от изменения стоимости ценных бумаг, оцениваемых по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка (сумма строк 30, 31)</t>
-  </si>
-  <si>
-    <t>Доходы от изменения справедливой стоимости финансовых инвестиций, оцениваемых по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка</t>
-  </si>
-  <si>
-    <t>Расходы от изменения справедливой стоимости финансовых инвестиций, оцениваемых по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка</t>
-  </si>
-  <si>
-    <t>Доходы (расходы) от изменения стоимости ценных бумаг, имеющихся в наличии для продажи (сумма строк 33-36)</t>
-  </si>
-  <si>
-    <t>Доходы от изменения справедливой стоимости краткосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Доходы от изменения справедливой стоимости долгосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Расходы от изменения справедливой стоимости краткосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Расходы от изменения справедливой стоимости долгосрочных финансовых инвестиций, имеющихся в наличии для продажи</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Расходы в виде вознаграждения по приобретенным ценным бумагам (сумма строк 38-41) </t>
-  </si>
-  <si>
-    <t>Расходы по амортизации премии по приобретенным краткосрочным финансовым инвестициям, удерживаемым до погашения</t>
-  </si>
-  <si>
-    <t>Расходы по амортизации премии по приобретенным долгосрочным финансовым инвестициям, удерживаемым до погашения</t>
-  </si>
-  <si>
-    <t>Расходы по амортизации премии по приобретенным краткосрочным финансовым инвестициям, имеющимся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Расходы по амортизации премии по приобретенным долгосрочным финансовым инвестициям, имеющимся в наличии для продажи</t>
-  </si>
-  <si>
-    <t>Расходы в виде вознаграждения по полученным займам и финансовой аренде (сумма строк 43-53)</t>
-  </si>
-  <si>
     <t>Расходы по вознаграждениям по краткосрочным банковским займам</t>
   </si>
   <si>
     <t>Расходы по вознаграждениям по долгосрочным банковским займам</t>
   </si>
   <si>
-    <t>Расходы по вознаграждениям по краткосрочным займам, полученным от организаций, осуществляющих банковские операции, без лицензии уполномоченного органа</t>
-  </si>
-  <si>
-    <t>Расходы по вознаграждениям по долгосрочным займам, полученным от организаций, осуществляющих банковские операции, без лицензии уполномоченного органа</t>
-  </si>
-  <si>
-    <t>Расходы по амортизации премии по краткосрочным предоставленным займам</t>
-  </si>
-  <si>
-    <t>Расходы по амортизации премии по долгосрочным предоставленным займам</t>
-  </si>
-  <si>
     <t>Расходы по амортизации дисконта по краткосрочным банковским займам полученным</t>
   </si>
   <si>
     <t>Расходы по амортизации дисконта по долгосрочным банковским займам полученным</t>
   </si>
   <si>
-    <t>Расходы по амортизации дисконта по краткосрочным займам, полученным от организаций, осуществляющих банковские операции, без лицензии уполномоченного органа</t>
-  </si>
-  <si>
-    <t>Расходы по амортизации дисконта по долгосрочным займам, полученным от организаций, осуществляющих банковские операции, без лицензии уполномоченного органа</t>
-  </si>
-  <si>
-    <t>Расходы на выплату процентов по финансовой аренде</t>
-  </si>
-  <si>
-    <t>ВСЕГО (сумма строк 1, 12, 22, 29, 32, 37 и 42)</t>
-  </si>
-  <si>
-    <t>* В гр.1 четвертый знак номера счета указывается с учетом принадлежности к контрагентам (эмитентам), то есть от 1 до 3</t>
-  </si>
-  <si>
     <t>** Доходы указываются со знаком плюс, расходы указываются со знаком минус. Увеличение доходов и уменьшение расходов указывается со знаком плюс, уменьшение доходов и увеличение расходов указывается со знаком минус.</t>
   </si>
   <si>
-    <t>*** Суммы, указанные в гр.5 и 7 по строкам 1, 12, 22, 29, 32, 37 и 42 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 2) по строкам 4, 5, 6, 7, 8, 11 и 12</t>
-  </si>
-  <si>
-    <t>**** Для КФГД суммы, указанные в гр.5 и 7 по строкам 1, 12, 22, 29, 32, 37 и 42 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 24) по строкам (5+16), (6+17), (7+18), (8+19), (9+20), (12+23) и (13+24)</t>
-  </si>
-  <si>
     <t>по состоянию на дату</t>
   </si>
   <si>
     <t>&lt;dd.MM.yyyy&gt;</t>
+  </si>
+  <si>
+    <t>Национальный идентификационный номер, международный идентификационный номер, наименование контрагента для вкладов и займов</t>
+  </si>
+  <si>
+    <t>Доходы в виде вознаграждения по размещенным вкладам (сумма строк 2-7)</t>
+  </si>
+  <si>
+    <t>Доходы в виде вознаграждения по приобретенным ценным бумагам (сумма строк 9-17)</t>
+  </si>
+  <si>
+    <t>Доходы по вознаграждениям по краткосрочным финансовым инвестициям, оцениваемым по справедливой стоимости через прибыль или убыток</t>
+  </si>
+  <si>
+    <t>Доходы по вознаграждениям по краткосрочным финансовым инвестициям, оцениваемым по амортизированной стоимости</t>
+  </si>
+  <si>
+    <t>Доходы по вознаграждениям по долгосрочным финансовым инвестициям, оцениваемым по амортизированной стоимости</t>
+  </si>
+  <si>
+    <t>Доходы по вознаграждениям по краткосрочным финансовым инвестициям, оцениваемым по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Доходы по вознаграждениям по долгосрочным финансовым инвестициям, оцениваемым по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Доходы по амортизации дисконта по краткосрочным финансовым инвестициям, оцениваемым по амортизированной стоимости</t>
+  </si>
+  <si>
+    <t>Доходы по амортизации дисконта по долгосрочным финансовым инвестициям, оцениваемым по амортизированной стоимости</t>
+  </si>
+  <si>
+    <t>Доходы по амортизации дисконта по краткосрочным финансовым инвестициям, оцениваемым по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Доходы по амортизации дисконта по долгосрочным финансовым инвестициям, оцениваемым по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Доходы в виде вознаграждения по заемным операциям (сумма строк 19-22)</t>
+  </si>
+  <si>
+    <t>Доходы по вознаграждению по краткосрочным заемным операциям</t>
+  </si>
+  <si>
+    <t>Доходы по вознаграждению по долгосрочным заемным операциям</t>
+  </si>
+  <si>
+    <t>Доходы по амортизации дисконта по краткосрочным заемным операциям</t>
+  </si>
+  <si>
+    <t>Доходы по амортизации дисконта по долгосрочным заемным операциям</t>
+  </si>
+  <si>
+    <t>Доходы (расходы) от купли-продажи ценных бумаг (сумма строк 24-29)</t>
+  </si>
+  <si>
+    <t>Доходы от покупки-продажи финансовых инвестиций, оцениваемых по справедливой стоимости через прибыль или убыток</t>
+  </si>
+  <si>
+    <t>Доходы от покупки-продажи краткосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Доходы от покупки-продажи долгосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Расходы от покупки-продажи финансовых инвестиций, оцениваемых по справедливой стоимости через прибыль или убыток</t>
+  </si>
+  <si>
+    <t>Расходы от покупки-продажи краткосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Расходы от покупки-продажи долгосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Доходы (расходы) от изменения стоимости ценных бумаг, оцениваемых по справедливой стоимости через прибыль или убыток (сумма строк 31,32)</t>
+  </si>
+  <si>
+    <t>Доходы от изменения справедливой стоимости финансовых инвестиций, оцениваемых по справедливой стоимости через прибыль или убыток</t>
+  </si>
+  <si>
+    <t>Расходы от изменения справедливой стоимости финансовых инвестиций, оцениваемых по справедливой стоимости через прибыль или убыток</t>
+  </si>
+  <si>
+    <t>Доходы (расходы) от изменения стоимости ценных бумаг, оцениваемых по справедливой стоимости через прочий совокупный доход (сумма строк 34-37)</t>
+  </si>
+  <si>
+    <t>Доходы от изменения справедливой стоимости краткосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Доходы от изменения справедливой стоимости долгосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Расходы от изменения справедливой стоимости краткосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Расходы от изменения справедливой стоимости долгосрочных финансовых инвестиций, оцениваемых по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Расходы в виде вознаграждения по приобретенным ценным бумагам (сумма строк 39-42) </t>
+  </si>
+  <si>
+    <t>Расходы по амортизации премии по приобретенным краткосрочным финансовым инвестициям, оцениваемым по амортизированной стоимости</t>
+  </si>
+  <si>
+    <t>Расходы по амортизации премии по приобретенным долгосрочным финансовым инвестициям, оцениваемым по амортизированной стоимости</t>
+  </si>
+  <si>
+    <t>Расходы по амортизации премии по приобретенным краткосрочным финансовым инвестициям, оцениваемым по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Расходы по амортизации премии по приобретенным долгосрочным финансовым инвестициям, оцениваемым по справедливой стоимости через прочий совокупный доход</t>
+  </si>
+  <si>
+    <t>Расходы в виде вознаграждения по заемным операциям и аренде (сумма строк 44-54)</t>
+  </si>
+  <si>
+    <t>Расходы по вознаграждениям по краткосрочным займам, полученным от юридических лиц за исключением банков второго уровня</t>
+  </si>
+  <si>
+    <t>Расходы по вознаграждениям по долгосрочным займам, полученным от юридических лиц за исключением банков второго уровня</t>
+  </si>
+  <si>
+    <t>Расходы по амортизации премии по краткосрочным заемным операциям</t>
+  </si>
+  <si>
+    <t>Расходы по амортизации премии по долгосрочным заемным операциям</t>
+  </si>
+  <si>
+    <t>Расходы по амортизации дисконта по краткосрочным займам, полученным от юридических лиц за исключением банков второго уровня</t>
+  </si>
+  <si>
+    <t>Расходы по амортизации дисконта по долгосрочным займам, полученным от юридических лиц за исключением банков второго уровня</t>
+  </si>
+  <si>
+    <t>Расходы на выплату процентов по аренде</t>
+  </si>
+  <si>
+    <t>Всего (сумма строк 1, 8, 18, 23, 30, 33, 38 и 43)</t>
+  </si>
+  <si>
+    <t>Примечание:* В гр.1 четвертый знак номера счета указывается с учетом принадлежности к контрагентам (эмитентам), то есть от 1 до 3</t>
+  </si>
+  <si>
+    <t>*** Суммы, указанные в гр.5 и 7 по строкам 1, 8, 18, 23, 30, 33, 38 и 43 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 2) по строкам 4, 5, 6, 7, 8, 9, 12 и 13</t>
+  </si>
+  <si>
+    <t>**** Для КФГД суммы, указанные в гр.5 и 7 по строкам 1, 8, 18, 23, 30, 33, 38 и 43 должны совпадать с соответствующими суммами, указанными в Отчете о прибылях и убытках (Приложение 24) по строкам (5+17), (6+18), (7+19), (8+20), (9+21), (10+22), (13+25) и (14+26)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
-  </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +321,19 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -393,129 +395,86 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -830,10 +789,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,8 +1584,8 @@
         <v>3</v>
       </c>
       <c r="B2"/>
-      <c r="C2" s="36" t="s">
-        <v>77</v>
+      <c r="C2" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="D2" s="3"/>
       <c r="G2" s="2" t="s">
@@ -1687,26 +1646,26 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="A10" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
@@ -1717,808 +1676,829 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="17" t="s">
         <v>16</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
         <v>1</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="18">
         <v>2</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="18">
         <v>3</v>
       </c>
       <c r="D14" s="18">
         <v>4</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="18">
         <v>5</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="18">
         <v>6</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="18">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21" t="s">
+    <row r="15" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="20">
+        <v>1</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="18">
+        <v>2</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="22">
-        <v>1</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="23" t="s">
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="17">
-        <v>2</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="23" t="s">
+      <c r="C18" s="18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="17">
-        <v>3</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="23" t="s">
+      <c r="C19" s="18">
+        <v>5</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="17">
-        <v>4</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="23" t="s">
+      <c r="C20" s="18">
+        <v>6</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="17">
-        <v>5</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="23" t="s">
+      <c r="C21" s="18">
+        <v>7</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="20">
+        <v>8</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+    </row>
+    <row r="23" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="18">
+        <v>9</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="18">
+        <v>10</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="18">
+        <v>11</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="18">
+        <v>12</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="18">
+        <v>13</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="18">
+        <v>14</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="18">
+        <v>15</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="18">
+        <v>16</v>
+      </c>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="18">
+        <v>17</v>
+      </c>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="20">
+        <v>18</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="18">
+        <v>19</v>
+      </c>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="18">
+        <v>20</v>
+      </c>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="18">
+        <v>21</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="18">
+        <v>22</v>
+      </c>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="20">
         <v>23</v>
       </c>
-      <c r="C20" s="17">
-        <v>6</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="23" t="s">
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="18">
         <v>24</v>
       </c>
-      <c r="C21" s="17">
-        <v>7</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="23" t="s">
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="18">
         <v>25</v>
       </c>
-      <c r="C22" s="17">
-        <v>8</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="23" t="s">
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="18">
         <v>26</v>
       </c>
-      <c r="C23" s="17">
-        <v>9</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="23" t="s">
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="18">
         <v>27</v>
       </c>
-      <c r="C24" s="17">
-        <v>10</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="23" t="s">
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="18">
         <v>28</v>
       </c>
-      <c r="C25" s="17">
-        <v>11</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="24" t="s">
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="18">
         <v>29</v>
       </c>
-      <c r="C26" s="22">
-        <v>12</v>
-      </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="25" t="s">
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="20">
         <v>30</v>
       </c>
-      <c r="C27" s="17">
-        <v>13</v>
-      </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="25" t="s">
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="18">
         <v>31</v>
       </c>
-      <c r="C28" s="17">
-        <v>14</v>
-      </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="25" t="s">
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+    </row>
+    <row r="46" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="18">
         <v>32</v>
       </c>
-      <c r="C29" s="17">
-        <v>15</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="25" t="s">
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="20">
         <v>33</v>
       </c>
-      <c r="C30" s="17">
-        <v>16</v>
-      </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="25" t="s">
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+    </row>
+    <row r="48" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="18">
         <v>34</v>
       </c>
-      <c r="C31" s="17">
-        <v>17</v>
-      </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="25" t="s">
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+    </row>
+    <row r="49" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="18">
         <v>35</v>
       </c>
-      <c r="C32" s="17">
-        <v>18</v>
-      </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="25" t="s">
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+    </row>
+    <row r="50" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="18">
         <v>36</v>
       </c>
-      <c r="C33" s="17">
-        <v>19</v>
-      </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="25" t="s">
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="18">
         <v>37</v>
       </c>
-      <c r="C34" s="17">
-        <v>20</v>
-      </c>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-    </row>
-    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="25" t="s">
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="20">
         <v>38</v>
       </c>
-      <c r="C35" s="17">
-        <v>21</v>
-      </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21" t="s">
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="18">
         <v>39</v>
       </c>
-      <c r="C36" s="22">
-        <v>22</v>
-      </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-    </row>
-    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="23" t="s">
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+    </row>
+    <row r="54" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="18">
         <v>40</v>
       </c>
-      <c r="C37" s="17">
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+    </row>
+    <row r="55" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="18">
+        <v>41</v>
+      </c>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+    </row>
+    <row r="56" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56" s="18">
+        <v>42</v>
+      </c>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+    </row>
+    <row r="57" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
+      <c r="B57" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="20">
+        <v>43</v>
+      </c>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+    </row>
+    <row r="58" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-    </row>
-    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-      <c r="B38" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="17">
+      <c r="C58" s="18">
+        <v>44</v>
+      </c>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+    </row>
+    <row r="59" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-    </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="17">
+      <c r="C59" s="18">
+        <v>45</v>
+      </c>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+    </row>
+    <row r="60" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="18">
+        <v>46</v>
+      </c>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+    </row>
+    <row r="61" spans="1:7" ht="39" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="18">
+        <v>47</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+    </row>
+    <row r="62" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="18">
+        <v>48</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="18">
+        <v>49</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+    </row>
+    <row r="64" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="20"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="28"/>
-    </row>
-    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="17">
+      <c r="C64" s="18">
+        <v>50</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+    </row>
+    <row r="65" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="17">
+      <c r="C65" s="18">
+        <v>51</v>
+      </c>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="21"/>
+    </row>
+    <row r="66" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="18">
+        <v>52</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+    </row>
+    <row r="67" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="18">
+        <v>53</v>
+      </c>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="18">
+        <v>54</v>
+      </c>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="25"/>
+      <c r="C69" s="20">
+        <v>55</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="17">
-        <v>28</v>
-      </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="28"/>
-    </row>
-    <row r="43" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="22">
-        <v>29</v>
-      </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-    </row>
-    <row r="44" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="17">
-        <v>30</v>
-      </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-    </row>
-    <row r="45" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="17">
-        <v>31</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-    </row>
-    <row r="46" spans="1:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="22">
-        <v>32</v>
-      </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="I46" s="29"/>
-    </row>
-    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="17">
-        <v>33</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="20"/>
-    </row>
-    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="17">
-        <v>34</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
-    </row>
-    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="17">
-        <v>35</v>
-      </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="20"/>
-    </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="17">
-        <v>36</v>
-      </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
-    </row>
-    <row r="51" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="22">
-        <v>37</v>
-      </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="20"/>
-    </row>
-    <row r="52" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="17">
-        <v>38</v>
-      </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="20"/>
-    </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="17">
-        <v>39</v>
-      </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="20"/>
-    </row>
-    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="17">
-        <v>40</v>
-      </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="20"/>
-    </row>
-    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="17">
-        <v>41</v>
-      </c>
-      <c r="D55" s="20"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="20"/>
-    </row>
-    <row r="56" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
-      <c r="B56" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="22">
-        <v>42</v>
-      </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
-    </row>
-    <row r="57" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="17">
-        <v>43</v>
-      </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-    </row>
-    <row r="58" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
-      <c r="B58" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="17">
-        <v>44</v>
-      </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-    </row>
-    <row r="59" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
-      <c r="B59" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="17">
-        <v>45</v>
-      </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="20"/>
-    </row>
-    <row r="60" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
-      <c r="B60" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="17">
-        <v>46</v>
-      </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="20"/>
-    </row>
-    <row r="61" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
-      <c r="B61" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="17">
-        <v>47</v>
-      </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="20"/>
-    </row>
-    <row r="62" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
-      <c r="B62" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="17">
-        <v>48</v>
-      </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="20"/>
-    </row>
-    <row r="63" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="17">
-        <v>49</v>
-      </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="20"/>
-    </row>
-    <row r="64" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
-      <c r="B64" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="17">
-        <v>50</v>
-      </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="20"/>
-    </row>
-    <row r="65" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="17">
-        <v>51</v>
-      </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="20"/>
-    </row>
-    <row r="66" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
-      <c r="B66" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" s="17">
-        <v>52</v>
-      </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="20"/>
-    </row>
-    <row r="67" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
-      <c r="B67" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="17">
-        <v>53</v>
-      </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="20"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="43"/>
-      <c r="C68" s="22">
-        <v>54</v>
-      </c>
-      <c r="D68" s="20"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="I68" s="29"/>
-    </row>
-    <row r="70" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="C70" s="45"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-    </row>
-    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="34"/>
-      <c r="B71" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="C71" s="45"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-    </row>
-    <row r="72" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
-      <c r="B72" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
-      <c r="G72" s="39"/>
-    </row>
-    <row r="73" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
-      <c r="B73" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B73:G73"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="A74:G74"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>

</xml_diff>